<commit_message>
greenhouse 7 inventory updated
</commit_message>
<xml_diff>
--- a/Planning/planning_2017/Greenhouse_7_postplanting_inventory.xlsx
+++ b/Planning/planning_2017/Greenhouse_7_postplanting_inventory.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/wildhellgarden/Planning/planning_2017/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="7780" yWindow="3780" windowWidth="40140" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -102,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>VIBCAS</t>
   </si>
@@ -198,24 +206,6 @@
   </si>
   <si>
     <t>TOTAL</t>
-  </si>
-  <si>
-    <t>Dan's notes:</t>
-  </si>
-  <si>
-    <t>1 DIELON_SH to plot 7</t>
-  </si>
-  <si>
-    <t>1 MYRGAL_GR to plot 8</t>
-  </si>
-  <si>
-    <t>1 MYRGAL_WM to plot 11</t>
-  </si>
-  <si>
-    <t>1 SPIALB_WM to plot 11</t>
-  </si>
-  <si>
-    <t>2 SPITOM_SH to plot 11</t>
   </si>
   <si>
     <t>AMECAN_SH in plot 12</t>
@@ -336,6 +326,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -664,17 +659,17 @@
   <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="25" max="25" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -749,30 +744,30 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B2">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>20</v>
       </c>
       <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
         <v>9</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>11</v>
-      </c>
       <c r="H2">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -784,13 +779,13 @@
         <v>46</v>
       </c>
       <c r="L2">
+        <v>8</v>
+      </c>
+      <c r="M2">
         <v>10</v>
       </c>
-      <c r="M2">
-        <v>12</v>
-      </c>
       <c r="N2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -799,7 +794,7 @@
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -811,7 +806,7 @@
         <v>0</v>
       </c>
       <c r="U2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -826,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -834,7 +829,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -849,7 +844,7 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -867,10 +862,10 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O3">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -879,7 +874,7 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S3">
         <v>10</v>
@@ -903,15 +898,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B4">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -920,7 +915,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -929,7 +924,7 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -938,19 +933,19 @@
         <v>15</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="N4">
         <v>0</v>
       </c>
       <c r="O4">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -968,7 +963,7 @@
         <v>0</v>
       </c>
       <c r="V4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W4">
         <v>0</v>
@@ -980,30 +975,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B5">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F5">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I5">
         <v>2</v>
@@ -1015,7 +1010,7 @@
         <v>28</v>
       </c>
       <c r="L5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -1057,7 +1052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -1134,7 +1129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -1211,7 +1206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -1288,17 +1283,17 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B9">
         <f t="shared" ref="B9:Y9" si="0">B2+B3+B4+B5+B6+B7+B8</f>
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
@@ -1306,23 +1301,23 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
@@ -1334,130 +1329,95 @@
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="M9">
         <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="0"/>
+        <v>109</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>36</v>
       </c>
-      <c r="N9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="R9">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="S9">
-        <f t="shared" si="0"/>
-        <v>109</v>
-      </c>
-      <c r="T9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="U9">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="V9">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="W9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="X9">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="Y9">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
     </row>
-    <row r="14" spans="1:25">
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25">
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25">
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="B19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="F20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="F21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="F22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="B23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="B24" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>